<commit_message>
temine de hacer la estadistica descriptva de las variables, hay algunas que por el formato de la pregunta hay que realizarle modificaciones para poder analizarlas.
</commit_message>
<xml_diff>
--- a/20211013_Encuesta a Turistas Pinto modificada.xlsx
+++ b/20211013_Encuesta a Turistas Pinto modificada.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\Observatorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\Observatorio\practica_diego\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7CB932-4FEB-45CD-B57F-6B051D176299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35487C7-5007-4D1F-8B5D-FEC055B027C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15525" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2265" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Encuestas" sheetId="2" r:id="rId1"/>
@@ -2467,12 +2467,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2487,7 +2493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2515,6 +2521,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2742,9 +2749,9 @@
   </sheetPr>
   <dimension ref="A1:BW179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="BS1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BW23" sqref="BW23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -2823,39 +2830,39 @@
         <v>752</v>
       </c>
       <c r="T1" s="9"/>
-      <c r="U1" s="9" t="s">
+      <c r="U1" s="13" t="s">
         <v>787</v>
       </c>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9" t="s">
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13" t="s">
         <v>788</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="13" t="s">
         <v>789</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="13" t="s">
         <v>753</v>
       </c>
       <c r="AA1" s="9" t="s">
         <v>790</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="13" t="s">
         <v>791</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="13" t="s">
         <v>792</v>
       </c>
       <c r="AD1" s="9" t="s">
         <v>793</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="13" t="s">
         <v>754</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="13" t="s">
         <v>755</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="13" t="s">
         <v>756</v>
       </c>
       <c r="AH1" s="9" t="s">
@@ -2897,7 +2904,7 @@
       <c r="AT1" s="9" t="s">
         <v>769</v>
       </c>
-      <c r="AU1" s="9" t="s">
+      <c r="AU1" s="13" t="s">
         <v>770</v>
       </c>
       <c r="AV1" s="9" t="s">
@@ -2912,26 +2919,26 @@
       <c r="AY1" s="9" t="s">
         <v>774</v>
       </c>
-      <c r="AZ1" s="9" t="s">
+      <c r="AZ1" s="13" t="s">
         <v>794</v>
       </c>
-      <c r="BA1" s="9" t="s">
+      <c r="BA1" s="13" t="s">
         <v>795</v>
       </c>
-      <c r="BB1" s="9"/>
-      <c r="BC1" s="9"/>
-      <c r="BD1" s="9"/>
-      <c r="BE1" s="9"/>
-      <c r="BF1" s="9"/>
-      <c r="BG1" s="9"/>
-      <c r="BH1" s="9" t="s">
+      <c r="BB1" s="13"/>
+      <c r="BC1" s="13"/>
+      <c r="BD1" s="13"/>
+      <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="13"/>
+      <c r="BH1" s="13" t="s">
         <v>796</v>
       </c>
-      <c r="BI1" s="9" t="s">
+      <c r="BI1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BJ1" s="9"/>
-      <c r="BK1" s="9"/>
+      <c r="BJ1" s="13"/>
+      <c r="BK1" s="13"/>
       <c r="BL1" s="9" t="s">
         <v>775</v>
       </c>
@@ -2965,7 +2972,7 @@
       <c r="BV1" s="9" t="s">
         <v>797</v>
       </c>
-      <c r="BW1" s="9" t="s">
+      <c r="BW1" s="13" t="s">
         <v>798</v>
       </c>
     </row>

</xml_diff>